<commit_message>
cleaning up extra info sheet
</commit_message>
<xml_diff>
--- a/assets/data/ToolExtraInfo.xlsx
+++ b/assets/data/ToolExtraInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faridah\Desktop\Research\Anonymous\website\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369DC22B-2559-406B-9914-E05ECCFD4A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E09560-781C-49BC-99E4-1CB344D1ECEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4F74CB56-8CE3-4D39-A187-8F2A5BC1EF5F}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
   <si>
     <t>FuzzDroid</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>ConDroid</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>Snowdrop</t>
   </si>
   <si>
-    <t>Usman et al.</t>
-  </si>
-  <si>
     <t>Availability</t>
   </si>
   <si>
@@ -154,6 +148,21 @@
   </si>
   <si>
     <t>Unspecified</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>COBWEB</t>
+  </si>
+  <si>
+    <t>Source code</t>
   </si>
 </sst>
 </file>
@@ -524,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6869538A-7598-479C-8430-7B52544476E0}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,29 +548,33 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3">
         <v>2014</v>
@@ -569,16 +582,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3">
         <v>2018</v>
@@ -586,16 +599,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="3">
         <v>2014</v>
@@ -603,14 +616,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E5" s="3">
         <v>2022</v>
@@ -618,12 +633,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3">
         <v>2023</v>
@@ -631,44 +650,50 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="E7" s="3">
-        <v>2014</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E8" s="3">
-        <v>2016</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3">
         <v>2016</v>
@@ -676,157 +701,169 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="3">
-        <v>2022</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E11" s="3">
-        <v>2018</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="E12" s="3">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E13" s="3">
-        <v>2013</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="D14" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E14" s="3">
-        <v>2016</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E15" s="3">
-        <v>2020</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="3">
-        <v>2017</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="3">
-        <v>2015</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="C18" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="3">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E19" s="3">
         <v>2016</v>
@@ -834,115 +871,135 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="E20" s="3">
-        <v>2014</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="C21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="E21" s="3">
-        <v>2017</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C22" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E22" s="3">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E23" s="3">
-        <v>2009</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="C24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E24" s="3">
-        <v>2014</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C25" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="E25" s="3">
-        <v>2020</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C26" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E26" s="3">
-        <v>2017</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E27" s="3">
         <v>2017</v>
@@ -950,13 +1007,19 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E28" s="3">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more data cleanup + rephrasing
</commit_message>
<xml_diff>
--- a/assets/data/ToolExtraInfo.xlsx
+++ b/assets/data/ToolExtraInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faridah\Desktop\Research\Anonymous\website\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56B94A0-1B0C-4884-8289-652C6B4C3F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953EC76E-9AA5-4DF1-AEBF-EBB04929CED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4F74CB56-8CE3-4D39-A187-8F2A5BC1EF5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="45">
   <si>
     <t>FuzzDroid</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>COLUMBUS</t>
-  </si>
-  <si>
-    <t>Frame</t>
   </si>
   <si>
     <t>Auto</t>
@@ -533,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6869538A-7598-479C-8430-7B52544476E0}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,13 +548,13 @@
         <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>24</v>
@@ -568,10 +565,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>25</v>
@@ -585,13 +582,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3">
         <v>2018</v>
@@ -619,13 +616,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="E5" s="3">
         <v>2022</v>
@@ -636,10 +633,10 @@
         <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>25</v>
@@ -650,16 +647,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E7" s="3">
         <v>2019</v>
@@ -670,10 +667,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>25</v>
@@ -687,13 +684,13 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="3">
         <v>2016</v>
@@ -704,10 +701,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>25</v>
@@ -721,10 +718,10 @@
         <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>25</v>
@@ -738,13 +735,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3">
         <v>2018</v>
@@ -755,7 +752,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>27</v>
@@ -772,13 +769,13 @@
         <v>18</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="3">
         <v>2013</v>
@@ -789,13 +786,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3">
         <v>2016</v>
@@ -806,10 +803,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>25</v>
@@ -823,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>27</v>
@@ -840,7 +837,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>27</v>
@@ -857,7 +854,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>27</v>
@@ -874,13 +871,13 @@
         <v>3</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="3">
         <v>2016</v>
@@ -891,13 +888,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="3">
         <v>2014</v>
@@ -905,16 +902,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="3">
         <v>2017</v>
@@ -922,16 +919,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="3">
         <v>2019</v>
@@ -942,13 +939,13 @@
         <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="E24" s="3">
         <v>2009</v>
@@ -959,13 +956,13 @@
         <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="3">
         <v>2014</v>
@@ -976,10 +973,10 @@
         <v>7</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>25</v>
@@ -993,10 +990,10 @@
         <v>12</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>25</v>
@@ -1007,13 +1004,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>25</v>

</xml_diff>